<commit_message>
Added one more fake result for demo. Added SpotId to results query. Fixed tests
</commit_message>
<xml_diff>
--- a/models/mock-data/Results.xlsx
+++ b/models/mock-data/Results.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="-1440" windowWidth="38400" windowHeight="21140" tabRatio="500"/>
+    <workbookView xWindow="28800" yWindow="-1440" windowWidth="38400" windowHeight="21060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="42">
   <si>
     <t>I3</t>
   </si>
@@ -141,6 +141,15 @@
   </si>
   <si>
     <t>Tyree.611</t>
+  </si>
+  <si>
+    <t>Mungo.80</t>
+  </si>
+  <si>
+    <t>I2</t>
+  </si>
+  <si>
+    <t>Great 8 to 5. Triple box TTR could use some work. Needs more intensity. Sloopy unstable. Playing inconsistent at best</t>
   </si>
 </sst>
 </file>
@@ -469,10 +478,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -739,6 +748,29 @@
         <v>11</v>
       </c>
     </row>
+    <row r="12" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="2">
+        <v>2</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>